<commit_message>
Add gcamp_type and expt_group
Add these two columns to Info and record in data.mat
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ignore</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>gcamp_type</t>
+  </si>
+  <si>
+    <t>expt_group</t>
+  </si>
+  <si>
+    <t>NDNF</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +470,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +525,11 @@
       <c r="R1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -568,6 +577,9 @@
       </c>
       <c r="R2" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>